<commit_message>
modify abstraction, discussion, conclusion
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wxing/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wxing/Desktop/alignment_free_network_comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>Linear :</t>
   </si>
@@ -168,13 +168,25 @@
   </si>
   <si>
     <t>GNB</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Experiment 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +203,22 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,8 +256,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -244,7 +274,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -255,6 +287,1059 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$O$6:$P$35</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="30"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>G1+space</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>G2+space</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>G3+space</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>G4+space</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>G5+space</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>G1+z</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>G2+z</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>G3+z</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>G4+z</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>G5+z</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>G1+space</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>G2+space</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>G3+space</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>G4+space</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>G5+space</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>G1+z</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>G2+z</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>G3+z</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>G4+z</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>G5+z</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>G1+space</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>G2+space</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>G3+space</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>G4+space</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>G5+space</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>G1+z</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>G2+z</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>G3+z</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>G4+z</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>G5+z</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>linear</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>RBF</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>GNB</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$6:$Q$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2067061440"/>
+        <c:axId val="-2119792992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2067061440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2119792992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2119792992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2067061440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,15 +1605,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:K41"/>
+  <dimension ref="A3:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,8 +1631,17 @@
       <c r="K5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -559,8 +1658,15 @@
       <c r="K6" s="3">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O6" s="3"/>
+      <c r="P6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -577,8 +1683,15 @@
       <c r="K7" s="3">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -597,8 +1710,17 @@
       <c r="K8" s="3">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -615,8 +1737,15 @@
       <c r="K9" s="3">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -633,8 +1762,15 @@
       <c r="K10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O10" s="3"/>
+      <c r="P10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
@@ -649,8 +1785,15 @@
       <c r="K11" s="3">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,8 +1810,15 @@
       <c r="K12" s="3">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -685,8 +1835,15 @@
       <c r="K13" s="3">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O13" s="3"/>
+      <c r="P13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -703,8 +1860,15 @@
       <c r="K14" s="3">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O14" s="3"/>
+      <c r="P14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -721,8 +1885,15 @@
       <c r="K15" s="4">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O15" s="4"/>
+      <c r="P15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -739,8 +1910,15 @@
       <c r="K16" s="5">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O16" s="5"/>
+      <c r="P16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="G17" s="3" t="s">
         <v>46</v>
@@ -757,8 +1935,17 @@
       <c r="K17" s="3">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -775,8 +1962,15 @@
       <c r="K18" s="3">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O18" s="3"/>
+      <c r="P18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -793,8 +1987,15 @@
       <c r="K19" s="3">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O19" s="3"/>
+      <c r="P19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -811,8 +2012,15 @@
       <c r="K20" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O20" s="3"/>
+      <c r="P20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -829,8 +2037,15 @@
       <c r="K21" s="3">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O21" s="3"/>
+      <c r="P21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
@@ -847,8 +2062,15 @@
       <c r="K22" s="3">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O22" s="3"/>
+      <c r="P22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
@@ -863,8 +2085,15 @@
       <c r="K23" s="3">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O23" s="3"/>
+      <c r="P23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -881,8 +2110,15 @@
       <c r="K24" s="3">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O24" s="3"/>
+      <c r="P24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -899,8 +2135,15 @@
       <c r="K25" s="3">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O25" s="3"/>
+      <c r="P25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
@@ -917,8 +2160,15 @@
       <c r="K26" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O26" s="3"/>
+      <c r="P26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
@@ -935,8 +2185,15 @@
       <c r="K27" s="4">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O27" s="4"/>
+      <c r="P27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -955,8 +2212,17 @@
       <c r="K28">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O28" t="s">
+        <v>47</v>
+      </c>
+      <c r="P28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="H29" t="s">
         <v>38</v>
@@ -970,8 +2236,14 @@
       <c r="K29">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P29" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q29">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>21</v>
       </c>
@@ -987,8 +2259,14 @@
       <c r="K30">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P30" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q30">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -1004,8 +2282,14 @@
       <c r="K31">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P31" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q31">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
@@ -1021,8 +2305,14 @@
       <c r="K32">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P32" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
@@ -1038,8 +2328,14 @@
       <c r="K33">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P33" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q33">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -1055,8 +2351,14 @@
       <c r="K34">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P34" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q34">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
@@ -1072,36 +2374,43 @@
       <c r="K35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P35" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>